<commit_message>
some fixes and adding latex support files
</commit_message>
<xml_diff>
--- a/data/vax_rollout.xlsx
+++ b/data/vax_rollout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monicarobles/Desktop/vac/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafa/myDocuments/projects/casos-vacunados-pr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B41185B-3427-6D4A-A166-CA86A977C40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E5FAC1-FD43-9246-96B6-51E88F6E7843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="960" windowWidth="28040" windowHeight="15840" xr2:uid="{8824D639-DEC9-3A4C-B8A7-E100784B6119}"/>
+    <workbookView xWindow="1100" yWindow="960" windowWidth="43320" windowHeight="16940" xr2:uid="{8824D639-DEC9-3A4C-B8A7-E100784B6119}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -42,40 +41,37 @@
     <t>What happened?</t>
   </si>
   <si>
-    <t>Johnson &amp; Johnson EUA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccine rollout is expanded to include everyone 16 years and older. </t>
-  </si>
-  <si>
-    <t>Moderna's EUA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDC reccomends vaccination for people 12 years and older. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The COVID-19 vaccine rollout begins with phase 1A which included   healthcare workers, communities in long term care facilities   and communities intelectual disabilities care facilities. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase 1B commences with the vaccination of adults 65 years and  older. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secretary of Health, Dr. Carlos Mellado, signs administrative order  estabiblishing that for the next 28 days, vaccination will be  exclusive for those 65 years and older. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">On March 3rd, 2021, Secretary of Health Dr. Carlos Mellado, signs  administrative order estabiblishing that starting on March 11th  and for the following 30 days, first doses are to be administered  exclusively to adults 60 years and older with certain cronic  conditions. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">On March 10th, 2021, Secretary of Health Dr. Carlos Mellado, signs   administrative order estabiblishing that starting on March 11th  and for the following 30 days, first doses are to be administered  exclusively to adults 60 years and older and 50 to 59 years olds  with  cronic conditions. </t>
-  </si>
-  <si>
-    <t>Secretary of Health signs executive order authorizing the   vaccination of personel in food industry, drug companies, medical  equipment, the public transport sector, air transport and   maritime cargo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase 1C begins with the vaccination of people 50 years and older  and 35 and older with cronic conditions. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase 2 begins with vaccination available to everyone  16 years and older. </t>
+    <t xml:space="preserve">CDC recommends vaccination for people 12 years and older. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The COVID-19 vaccine rollout begins with phase 1A which included  healthcare workers, communities in long term care facilities and intellectual disabilities care facilities. </t>
+  </si>
+  <si>
+    <t>mRNA-1273 (Moderna) receive Emergency Use Authorization (EUA).</t>
+  </si>
+  <si>
+    <t>Ad26.COV2.S (Johnson &amp; Johnson) recieves EUA</t>
+  </si>
+  <si>
+    <t>Secretary of Health signs executive order authorizing the  vaccination of personnel in food industry, drug companies, medical  equipment, the public transport sector, air transport and   maritime cargo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 1C begins with the vaccination of people 50 and older  and 35 and older with chronic conditions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 1B commences with the vaccination of adults 65 and  older. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerto Rico's Secretary of Health signs administrative order establishing that for the next 28 days, vaccination will be  exclusive for those 65 and older. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On March 3rd, 2021 Secretary of Health  signs  administrative order establishing that starting on March 11th  and for the following 30 days, first doses are to be administered exclusively to adults 60 and older with certain chronic conditions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On March 10th, 2021,  Secretary signs  administrative order establishing that starting on March 11th  and for the following 30 days, first doses are to be administered  exclusively to adults 60 and older and 50 to 59 year olds  with  chronic conditions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 2 begins with vaccination available to everyone 16 and older. </t>
   </si>
 </sst>
 </file>
@@ -83,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -119,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,16 +430,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F86457-EA73-F54D-AF46-DFDB8BAC705D}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="2" max="2" width="172.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,12 +450,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44180</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -470,20 +466,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44207</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44229</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -491,63 +487,55 @@
         <v>44258</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44266</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44267</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44272</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44284</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44298</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44302</v>
+        <v>44328</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>44328</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>